<commit_message>
[RCE] DT and SVM results up to 325000 rows
</commit_message>
<xml_diff>
--- a/project/ExperimentRecord - Target Variable - Acceptable_Resolution_Status.xlsx
+++ b/project/ExperimentRecord - Target Variable - Acceptable_Resolution_Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\school\SPS\DATA622\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5964362-EB17-4047-B14E-55E009E39045}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EB4B75-64B3-461F-9DD7-C7E33C26E70C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="1260" windowWidth="12825" windowHeight="8685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="495" yWindow="1620" windowWidth="12300" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Size</t>
   </si>
@@ -54,33 +54,9 @@
     <t>RF 3</t>
   </si>
   <si>
-    <t>Random Forest Accuracies</t>
-  </si>
-  <si>
-    <t>RF 3 ntree</t>
-  </si>
-  <si>
-    <t>seconds</t>
-  </si>
-  <si>
-    <t>minutes</t>
-  </si>
-  <si>
-    <t>Variable Size</t>
-  </si>
-  <si>
     <t>SVM</t>
   </si>
   <si>
-    <t>SVM Times</t>
-  </si>
-  <si>
-    <t>RF Times</t>
-  </si>
-  <si>
-    <t>SVM Tuning was on.</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -99,9 +75,6 @@
     <t>%NAs</t>
   </si>
   <si>
-    <t>O(n)</t>
-  </si>
-  <si>
     <t>SVM 1 - linear, gamma = 0.05, cost = 6</t>
   </si>
   <si>
@@ -111,13 +84,25 @@
     <t>SVM 3 - NOT EXECUTED - polynomial, could not even execute at size 400.</t>
   </si>
   <si>
-    <t>SVM Accuracies</t>
-  </si>
-  <si>
     <t>SVM 1</t>
   </si>
   <si>
     <t>SVM 2</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>Accuracies</t>
+  </si>
+  <si>
+    <t>Times (Minutes)</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>Var Size</t>
   </si>
 </sst>
 </file>
@@ -153,7 +138,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -300,17 +285,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,60 +571,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BE26"/>
+  <dimension ref="A1:BC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="7"/>
       <c r="K1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="L1" s="6"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -656,86 +631,78 @@
       <c r="G2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>26</v>
+      <c r="H2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="22"/>
-    </row>
-    <row r="3" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>400</v>
       </c>
       <c r="B3" s="2">
-        <f>A3-D3</f>
+        <f t="shared" ref="B3:B11" si="0">A3-D3</f>
         <v>90</v>
       </c>
-      <c r="C3" s="18">
-        <f>B3/A3</f>
+      <c r="C3" s="14">
+        <f t="shared" ref="C3:C16" si="1">B3/A3</f>
         <v>0.22500000000000001</v>
       </c>
       <c r="D3" s="3">
         <v>310</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="15">
         <v>0.89500000000000002</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="15">
         <v>0.89500000000000002</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="15">
         <v>0.89500000000000002</v>
       </c>
-      <c r="H3" s="3">
-        <v>500</v>
-      </c>
-      <c r="I3" s="19">
+      <c r="H3" s="15">
         <v>0.83299999999999996</v>
       </c>
-      <c r="J3" s="19">
+      <c r="I3" s="15">
         <v>0.97399999999999998</v>
       </c>
-      <c r="K3" s="3">
-        <v>4</v>
+      <c r="J3" s="16">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="K3" s="12">
+        <f>3.81/60</f>
+        <v>6.3500000000000001E-2</v>
       </c>
       <c r="L3" s="12">
-        <f>K3/60</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="M3" s="14">
-        <v>956</v>
-      </c>
-      <c r="N3" s="12">
-        <f>M3/60</f>
-        <v>15.933333333333334</v>
-      </c>
-      <c r="O3" s="3">
+        <f>0.98/60</f>
+        <v>1.6333333333333332E-2</v>
+      </c>
+      <c r="M3" s="18">
+        <f>0.53/60</f>
+        <v>8.8333333333333337E-3</v>
+      </c>
+      <c r="N3" s="3">
         <v>54</v>
       </c>
-      <c r="P3" s="3">
-        <f>LOG(M3,K3)</f>
-        <v>4.9504334039903739</v>
-      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -775,63 +742,57 @@
       <c r="BA3" s="1"/>
       <c r="BB3" s="1"/>
       <c r="BC3" s="1"/>
-      <c r="BD3" s="1"/>
-      <c r="BE3" s="1"/>
-    </row>
-    <row r="4" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>800</v>
       </c>
       <c r="B4" s="2">
-        <f>A4-D4</f>
+        <f t="shared" si="0"/>
         <v>232</v>
       </c>
-      <c r="C4" s="18">
-        <f>B4/A4</f>
+      <c r="C4" s="14">
+        <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="D4" s="2">
         <v>568</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="16">
         <v>0.96499999999999997</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="16">
         <v>0.97199999999999998</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="16">
         <v>0.96499999999999997</v>
       </c>
-      <c r="H4" s="2">
-        <v>400</v>
-      </c>
-      <c r="I4" s="20">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="J4" s="20">
+      <c r="H4" s="16">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="I4" s="16">
         <v>0.95099999999999996</v>
       </c>
-      <c r="K4" s="2">
-        <v>3</v>
+      <c r="J4" s="16">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="K4" s="12">
+        <f>3.14/60</f>
+        <v>5.2333333333333336E-2</v>
       </c>
       <c r="L4" s="12">
-        <f>K4/60</f>
-        <v>0.05</v>
-      </c>
-      <c r="M4" s="2">
-        <v>5.26</v>
-      </c>
-      <c r="N4" s="12">
-        <f>M4/60</f>
-        <v>8.7666666666666657E-2</v>
-      </c>
-      <c r="O4" s="2">
+        <f>0.89/60</f>
+        <v>1.4833333333333334E-2</v>
+      </c>
+      <c r="M4" s="18">
+        <f>0.56/60</f>
+        <v>9.3333333333333341E-3</v>
+      </c>
+      <c r="N4" s="2">
         <v>65</v>
       </c>
-      <c r="P4" s="2">
-        <f>LOG(M4,K4)</f>
-        <v>1.5111163818877902</v>
-      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -871,63 +832,57 @@
       <c r="BA4" s="1"/>
       <c r="BB4" s="1"/>
       <c r="BC4" s="1"/>
-      <c r="BD4" s="1"/>
-      <c r="BE4" s="1"/>
-    </row>
-    <row r="5" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1600</v>
       </c>
       <c r="B5" s="2">
-        <f>A5-D5</f>
+        <f t="shared" si="0"/>
         <v>433</v>
       </c>
-      <c r="C5" s="18">
-        <f>B5/A5</f>
+      <c r="C5" s="14">
+        <f t="shared" si="1"/>
         <v>0.270625</v>
       </c>
       <c r="D5" s="2">
         <v>1167</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="16">
         <v>0.94499999999999995</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="16">
         <v>0.94199999999999995</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="16">
         <v>0.94199999999999995</v>
       </c>
-      <c r="H5" s="2">
-        <v>300</v>
-      </c>
-      <c r="I5" s="20">
+      <c r="H5" s="16">
         <v>0.753</v>
       </c>
-      <c r="J5" s="20">
+      <c r="I5" s="16">
         <v>0.92900000000000005</v>
       </c>
-      <c r="K5" s="2">
-        <v>3.95</v>
+      <c r="J5" s="16">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="K5" s="12">
+        <f>4/60</f>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="L5" s="12">
-        <f>K5/60</f>
-        <v>6.5833333333333341E-2</v>
-      </c>
-      <c r="M5" s="15">
-        <v>3367</v>
-      </c>
-      <c r="N5" s="12">
-        <f>M5/60</f>
-        <v>56.116666666666667</v>
-      </c>
-      <c r="O5" s="2">
+        <f>1.12/60</f>
+        <v>1.8666666666666668E-2</v>
+      </c>
+      <c r="M5" s="18">
+        <f>0.58/60</f>
+        <v>9.6666666666666654E-3</v>
+      </c>
+      <c r="N5" s="2">
         <v>70</v>
       </c>
-      <c r="P5" s="2">
-        <f>LOG(M5,K5)</f>
-        <v>5.9122700097698022</v>
-      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -967,63 +922,57 @@
       <c r="BA5" s="1"/>
       <c r="BB5" s="1"/>
       <c r="BC5" s="1"/>
-      <c r="BD5" s="1"/>
-      <c r="BE5" s="1"/>
-    </row>
-    <row r="6" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3200</v>
       </c>
       <c r="B6" s="2">
-        <f>A6-D6</f>
+        <f t="shared" si="0"/>
         <v>853</v>
       </c>
-      <c r="C6" s="18">
-        <f>B6/A6</f>
+      <c r="C6" s="14">
+        <f t="shared" si="1"/>
         <v>0.26656249999999998</v>
       </c>
       <c r="D6" s="2">
         <v>2347</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="16">
         <v>0.94199999999999995</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="16">
         <v>0.94399999999999995</v>
       </c>
-      <c r="G6" s="20">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="H6" s="2">
-        <v>350</v>
-      </c>
-      <c r="I6" s="20">
+      <c r="G6" s="16">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="H6" s="16">
         <v>0.49399999999999999</v>
       </c>
-      <c r="J6" s="20">
+      <c r="I6" s="16">
         <v>0.93700000000000006</v>
       </c>
-      <c r="K6" s="2">
-        <v>6</v>
+      <c r="J6" s="16">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="K6" s="12">
+        <f>5.92/60</f>
+        <v>9.8666666666666666E-2</v>
       </c>
       <c r="L6" s="12">
-        <f>K6/60</f>
-        <v>0.1</v>
-      </c>
-      <c r="M6" s="2">
-        <v>21.99</v>
-      </c>
-      <c r="N6" s="12">
-        <f>M6/60</f>
-        <v>0.36649999999999999</v>
-      </c>
-      <c r="O6" s="2">
+        <f>21.87/60</f>
+        <v>0.36449999999999999</v>
+      </c>
+      <c r="M6" s="18">
+        <f>0.66/60</f>
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="N6" s="2">
         <v>75</v>
       </c>
-      <c r="P6" s="2">
-        <f>LOG(M6,K6)</f>
-        <v>1.7248898960183479</v>
-      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -1063,63 +1012,57 @@
       <c r="BA6" s="1"/>
       <c r="BB6" s="1"/>
       <c r="BC6" s="1"/>
-      <c r="BD6" s="1"/>
-      <c r="BE6" s="1"/>
-    </row>
-    <row r="7" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6400</v>
       </c>
       <c r="B7" s="2">
-        <f>A7-D7</f>
+        <f t="shared" si="0"/>
         <v>1709</v>
       </c>
-      <c r="C7" s="18">
-        <f>B7/A7</f>
+      <c r="C7" s="14">
+        <f t="shared" si="1"/>
         <v>0.26703125</v>
       </c>
       <c r="D7" s="2">
         <v>4691</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="16">
         <v>0.95</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="16">
         <v>0.94499999999999995</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="16">
         <v>0.94599999999999995</v>
       </c>
-      <c r="H7" s="2">
-        <v>400</v>
-      </c>
-      <c r="I7" s="20">
+      <c r="H7" s="16">
         <v>0.60399999999999998</v>
       </c>
-      <c r="J7" s="20">
+      <c r="I7" s="16">
         <v>0.95499999999999996</v>
       </c>
-      <c r="K7" s="2">
-        <v>9.8000000000000007</v>
+      <c r="J7" s="16">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="K7" s="12">
+        <f>9.65/60</f>
+        <v>0.16083333333333333</v>
       </c>
       <c r="L7" s="12">
-        <f>K7/60</f>
-        <v>0.16333333333333336</v>
-      </c>
-      <c r="M7" s="2">
-        <v>3.84</v>
-      </c>
-      <c r="N7" s="12">
-        <f>M7/60</f>
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="O7" s="2">
+        <f>3.69/60</f>
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="M7" s="18">
+        <f>0.83/60</f>
+        <v>1.3833333333333333E-2</v>
+      </c>
+      <c r="N7" s="2">
         <v>77</v>
       </c>
-      <c r="P7" s="2">
-        <f>LOG(M7,K7)</f>
-        <v>0.58950348330909541</v>
-      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -1159,63 +1102,57 @@
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
       <c r="BC7" s="1"/>
-      <c r="BD7" s="1"/>
-      <c r="BE7" s="1"/>
-    </row>
-    <row r="8" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>12800</v>
       </c>
       <c r="B8" s="2">
-        <f>A8-D8</f>
+        <f t="shared" si="0"/>
         <v>3597</v>
       </c>
-      <c r="C8" s="18">
-        <f>B8/A8</f>
+      <c r="C8" s="14">
+        <f t="shared" si="1"/>
         <v>0.28101562499999999</v>
       </c>
       <c r="D8" s="2">
         <v>9203</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="16">
         <v>0.94499999999999995</v>
       </c>
-      <c r="F8" s="20">
-        <v>0.94</v>
-      </c>
-      <c r="G8" s="20">
+      <c r="F8" s="16">
         <v>0.94099999999999995</v>
       </c>
-      <c r="H8" s="2">
-        <v>400</v>
-      </c>
-      <c r="I8" s="20">
+      <c r="G8" s="16">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="H8" s="16">
         <v>0.48299999999999998</v>
       </c>
-      <c r="J8" s="20">
+      <c r="I8" s="16">
         <v>0.93</v>
       </c>
-      <c r="K8" s="2">
-        <v>15.89</v>
+      <c r="J8" s="16">
+        <v>0.92</v>
+      </c>
+      <c r="K8" s="12">
+        <f>16.11/60</f>
+        <v>0.26850000000000002</v>
       </c>
       <c r="L8" s="12">
-        <f>K8/60</f>
-        <v>0.26483333333333337</v>
-      </c>
-      <c r="M8" s="2">
-        <v>18.22</v>
-      </c>
-      <c r="N8" s="12">
-        <f>M8/60</f>
-        <v>0.30366666666666664</v>
-      </c>
-      <c r="O8" s="2">
+        <f>18.26/60</f>
+        <v>0.30433333333333334</v>
+      </c>
+      <c r="M8" s="18">
+        <f>1.25/60</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="N8" s="2">
         <v>91</v>
       </c>
-      <c r="P8" s="2">
-        <f>LOG(M8,K8)</f>
-        <v>1.0494740597266961</v>
-      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1255,63 +1192,57 @@
       <c r="BA8" s="1"/>
       <c r="BB8" s="1"/>
       <c r="BC8" s="1"/>
-      <c r="BD8" s="1"/>
-      <c r="BE8" s="1"/>
-    </row>
-    <row r="9" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>25600</v>
       </c>
       <c r="B9" s="2">
-        <f>A9-D9</f>
+        <f t="shared" si="0"/>
         <v>7461</v>
       </c>
-      <c r="C9" s="18">
-        <f>B9/A9</f>
+      <c r="C9" s="14">
+        <f t="shared" si="1"/>
         <v>0.2914453125</v>
       </c>
       <c r="D9" s="2">
         <v>18139</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="16">
         <v>0.94399999999999995</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="16">
         <v>0.95099999999999996</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="16">
         <v>0.95099999999999996</v>
       </c>
-      <c r="H9" s="2">
-        <v>400</v>
-      </c>
-      <c r="I9" s="20">
+      <c r="H9" s="16">
         <v>0.54500000000000004</v>
       </c>
-      <c r="J9" s="20">
+      <c r="I9" s="16">
         <v>0.92400000000000004</v>
       </c>
-      <c r="K9" s="2">
-        <v>30.29</v>
+      <c r="J9" s="16">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="K9" s="12">
+        <f>30.3/60</f>
+        <v>0.505</v>
       </c>
       <c r="L9" s="12">
-        <f>K9/60</f>
-        <v>0.50483333333333336</v>
-      </c>
-      <c r="M9" s="2">
-        <v>48.36</v>
-      </c>
-      <c r="N9" s="12">
-        <f>M9/60</f>
+        <f>48.36/60</f>
         <v>0.80599999999999994</v>
       </c>
-      <c r="O9" s="2">
+      <c r="M9" s="18">
+        <f>1.97/60</f>
+        <v>3.2833333333333332E-2</v>
+      </c>
+      <c r="N9" s="2">
         <v>102</v>
       </c>
-      <c r="P9" s="2">
-        <f>LOG(M9,K9)</f>
-        <v>1.1371681081019618</v>
-      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -1351,68 +1282,62 @@
       <c r="BA9" s="1"/>
       <c r="BB9" s="1"/>
       <c r="BC9" s="1"/>
-      <c r="BD9" s="1"/>
-      <c r="BE9" s="1"/>
-    </row>
-    <row r="10" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>65000</v>
       </c>
       <c r="B10" s="2">
-        <f>A10-D10</f>
+        <f t="shared" si="0"/>
         <v>18047</v>
       </c>
-      <c r="C10" s="18">
-        <f>B10/A10</f>
+      <c r="C10" s="14">
+        <f t="shared" si="1"/>
         <v>0.27764615384615382</v>
       </c>
       <c r="D10" s="2">
         <v>46953</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="16">
         <v>0.94199999999999995</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="16">
         <v>0.95299999999999996</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="16">
         <v>0.95299999999999996</v>
       </c>
-      <c r="H10" s="2">
-        <v>420</v>
-      </c>
-      <c r="I10" s="20">
+      <c r="H10" s="16">
         <v>0.57999999999999996</v>
       </c>
-      <c r="J10" s="20">
+      <c r="I10" s="16">
         <v>0.92600000000000005</v>
       </c>
-      <c r="K10" s="2">
-        <v>83.57</v>
+      <c r="J10" s="16">
+        <v>0.93</v>
+      </c>
+      <c r="K10" s="12">
+        <f>83.86/60</f>
+        <v>1.3976666666666666</v>
       </c>
       <c r="L10" s="12">
-        <f>K10/60</f>
-        <v>1.3928333333333331</v>
-      </c>
-      <c r="M10" s="2">
-        <v>313.54000000000002</v>
-      </c>
-      <c r="N10" s="12">
-        <f>M10/60</f>
-        <v>5.2256666666666671</v>
-      </c>
-      <c r="O10" s="2">
+        <f>319.98/60</f>
+        <v>5.3330000000000002</v>
+      </c>
+      <c r="M10" s="18">
+        <f>5.16/60</f>
+        <v>8.6000000000000007E-2</v>
+      </c>
+      <c r="N10" s="2">
         <v>110</v>
       </c>
-      <c r="P10" s="2">
-        <f>LOG(M10,K10)</f>
-        <v>1.2987656053095133</v>
-      </c>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1">
+      <c r="O10" s="1"/>
+      <c r="P10" s="1">
         <f>195000*0.3</f>
         <v>58500</v>
       </c>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -1450,63 +1375,57 @@
       <c r="BA10" s="1"/>
       <c r="BB10" s="1"/>
       <c r="BC10" s="1"/>
-      <c r="BD10" s="1"/>
-      <c r="BE10" s="1"/>
-    </row>
-    <row r="11" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>130000</v>
       </c>
       <c r="B11" s="2">
-        <f>A11-D11</f>
+        <f t="shared" si="0"/>
         <v>37958</v>
       </c>
-      <c r="C11" s="18">
-        <f>B11/A11</f>
+      <c r="C11" s="14">
+        <f t="shared" si="1"/>
         <v>0.2919846153846154</v>
       </c>
       <c r="D11" s="2">
         <v>92042</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="16">
         <v>0.94099999999999995</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="16">
         <v>0.94799999999999995</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="16">
         <v>0.94799999999999995</v>
       </c>
-      <c r="H11" s="2">
-        <v>420</v>
-      </c>
-      <c r="I11" s="20">
+      <c r="H11" s="16">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J11" s="20">
+      <c r="I11" s="16">
         <v>0.91700000000000004</v>
       </c>
-      <c r="K11" s="2">
-        <v>183.31</v>
-      </c>
-      <c r="L11" s="13">
-        <f>K11/60</f>
-        <v>3.0551666666666666</v>
-      </c>
-      <c r="M11" s="2">
-        <v>2098</v>
-      </c>
-      <c r="N11" s="13">
-        <f>M11/60</f>
-        <v>34.966666666666669</v>
-      </c>
-      <c r="O11" s="2">
+      <c r="J11" s="16">
+        <v>0.91</v>
+      </c>
+      <c r="K11" s="12">
+        <f>182.24/60</f>
+        <v>3.0373333333333337</v>
+      </c>
+      <c r="L11" s="12">
+        <f>2143.99/60</f>
+        <v>35.733166666666662</v>
+      </c>
+      <c r="M11" s="18">
+        <f>9.99/60</f>
+        <v>0.16650000000000001</v>
+      </c>
+      <c r="N11" s="2">
         <v>117</v>
       </c>
-      <c r="P11" s="2">
-        <f>LOG(M11,K11)</f>
-        <v>1.4677561865496691</v>
-      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -1546,64 +1465,58 @@
       <c r="BA11" s="1"/>
       <c r="BB11" s="1"/>
       <c r="BC11" s="1"/>
-      <c r="BD11" s="1"/>
-      <c r="BE11" s="1"/>
-    </row>
-    <row r="12" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f>A11+65000</f>
+        <f t="shared" ref="A12:A17" si="2">A11+65000</f>
         <v>195000</v>
       </c>
       <c r="B12" s="2">
         <v>58456</v>
       </c>
-      <c r="C12" s="18">
-        <f>B12/A12</f>
+      <c r="C12" s="14">
+        <f t="shared" si="1"/>
         <v>0.299774358974359</v>
       </c>
       <c r="D12" s="2">
         <f>A12-B12</f>
         <v>136544</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="16">
         <v>0.93100000000000005</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="16">
         <v>0.94599999999999995</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="16">
         <v>0.94599999999999995</v>
       </c>
-      <c r="H12" s="2">
-        <v>420</v>
-      </c>
-      <c r="I12" s="20">
+      <c r="H12" s="16">
         <v>0.59</v>
       </c>
-      <c r="J12" s="20">
+      <c r="I12" s="16">
         <v>0.91500000000000004</v>
       </c>
-      <c r="K12" s="2">
-        <v>333.91</v>
+      <c r="J12" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="K12" s="12">
+        <f>330.43/60</f>
+        <v>5.5071666666666665</v>
       </c>
       <c r="L12" s="12">
-        <f>K12/60</f>
-        <v>5.5651666666666673</v>
-      </c>
-      <c r="M12" s="2">
-        <v>5036</v>
-      </c>
-      <c r="N12" s="12">
-        <f>M12/60</f>
-        <v>83.933333333333337</v>
-      </c>
-      <c r="O12" s="2">
+        <f>5087.87/60</f>
+        <v>84.79783333333333</v>
+      </c>
+      <c r="M12" s="18">
+        <f>16.7/60</f>
+        <v>0.27833333333333332</v>
+      </c>
+      <c r="N12" s="2">
         <v>123</v>
       </c>
-      <c r="P12" s="2">
-        <f>LOG(M12,K12)</f>
-        <v>1.4669688361955602</v>
-      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -1643,64 +1556,58 @@
       <c r="BA12" s="1"/>
       <c r="BB12" s="1"/>
       <c r="BC12" s="1"/>
-      <c r="BD12" s="1"/>
-      <c r="BE12" s="1"/>
-    </row>
-    <row r="13" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <f>A12+65000</f>
+        <f t="shared" si="2"/>
         <v>260000</v>
       </c>
       <c r="B13" s="2">
         <f>A13-D13</f>
         <v>76303</v>
       </c>
-      <c r="C13" s="23">
-        <f>B13/A13</f>
+      <c r="C13" s="17">
+        <f t="shared" si="1"/>
         <v>0.29347307692307695</v>
       </c>
       <c r="D13" s="2">
         <v>183697</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="16">
         <v>0.92700000000000005</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="16">
         <v>0.94399999999999995</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="16">
         <v>0.94399999999999995</v>
       </c>
-      <c r="H13" s="2">
-        <v>420</v>
-      </c>
-      <c r="I13" s="20">
+      <c r="H13" s="16">
         <v>0.51</v>
       </c>
-      <c r="J13" s="20">
+      <c r="I13" s="16">
         <v>0.91</v>
       </c>
-      <c r="K13" s="13">
-        <v>526.95000000000005</v>
-      </c>
-      <c r="L13" s="13">
-        <f>K13/60</f>
-        <v>8.7825000000000006</v>
-      </c>
-      <c r="M13" s="13">
-        <v>14329.04</v>
-      </c>
-      <c r="N13" s="13">
-        <f>M13/60</f>
-        <v>238.81733333333335</v>
-      </c>
-      <c r="O13" s="2">
+      <c r="J13" s="16">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="K13" s="12">
+        <f>522.28/60</f>
+        <v>8.7046666666666663</v>
+      </c>
+      <c r="L13" s="12">
+        <f>14093.59/60</f>
+        <v>234.89316666666667</v>
+      </c>
+      <c r="M13" s="18">
+        <f>22.37/60</f>
+        <v>0.37283333333333335</v>
+      </c>
+      <c r="N13" s="2">
         <v>125</v>
       </c>
-      <c r="P13" s="2">
-        <f>LOG(M13,K13)</f>
-        <v>1.527027631920435</v>
-      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -1740,14 +1647,56 @@
       <c r="BA13" s="1"/>
       <c r="BB13" s="1"/>
       <c r="BC13" s="1"/>
-      <c r="BD13" s="1"/>
-      <c r="BE13" s="1"/>
-    </row>
-    <row r="14" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f>A13+65000</f>
+        <f t="shared" si="2"/>
         <v>325000</v>
       </c>
+      <c r="B14" s="2">
+        <f>A14-D14</f>
+        <v>95505</v>
+      </c>
+      <c r="C14" s="17">
+        <f t="shared" si="1"/>
+        <v>0.29386153846153845</v>
+      </c>
+      <c r="D14" s="2">
+        <v>229495</v>
+      </c>
+      <c r="E14" s="16">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0.94</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0.94</v>
+      </c>
+      <c r="H14" s="16">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I14" s="16">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="12">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="18">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>125</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -1787,14 +1736,56 @@
       <c r="BA14" s="1"/>
       <c r="BB14" s="1"/>
       <c r="BC14" s="1"/>
-      <c r="BD14" s="1"/>
-      <c r="BE14" s="1"/>
-    </row>
-    <row r="15" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f>A14+65000</f>
+        <f t="shared" si="2"/>
         <v>390000</v>
       </c>
+      <c r="B15" s="2">
+        <f>A15-D15</f>
+        <v>113828</v>
+      </c>
+      <c r="C15" s="17">
+        <f t="shared" si="1"/>
+        <v>0.29186666666666666</v>
+      </c>
+      <c r="D15" s="2">
+        <v>276172</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0.91</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="12">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="18">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>128</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -1834,14 +1825,56 @@
       <c r="BA15" s="1"/>
       <c r="BB15" s="1"/>
       <c r="BC15" s="1"/>
-      <c r="BD15" s="1"/>
-      <c r="BE15" s="1"/>
-    </row>
-    <row r="16" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f>A15+65000</f>
+        <f t="shared" si="2"/>
         <v>455000</v>
       </c>
+      <c r="B16" s="2">
+        <f>A16-D16</f>
+        <v>130985</v>
+      </c>
+      <c r="C16" s="17">
+        <f t="shared" si="1"/>
+        <v>0.28787912087912088</v>
+      </c>
+      <c r="D16" s="2">
+        <v>324015</v>
+      </c>
+      <c r="E16" s="16">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="G16" s="16">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="H16" s="16">
+        <v>0.53</v>
+      </c>
+      <c r="I16" s="16">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="12">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="18">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>129</v>
+      </c>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -1881,31 +1914,36 @@
       <c r="BA16" s="1"/>
       <c r="BB16" s="1"/>
       <c r="BC16" s="1"/>
-      <c r="BD16" s="1"/>
-      <c r="BE16" s="1"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f>A16+65000</f>
+        <f t="shared" si="2"/>
         <v>520000</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="12">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="18">
+        <f>0/60</f>
+        <v>0</v>
+      </c>
       <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1920,47 +1958,40 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[RCE] Update all models for 520000 rows
</commit_message>
<xml_diff>
--- a/project/ExperimentRecord - Target Variable - Acceptable_Resolution_Status.xlsx
+++ b/project/ExperimentRecord - Target Variable - Acceptable_Resolution_Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\school\SPS\DATA622\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EB4B75-64B3-461F-9DD7-C7E33C26E70C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C4AD8B-F82A-4257-B7D8-A62ADE234CCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="1620" windowWidth="12300" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="600" windowWidth="12300" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +662,7 @@
         <v>90</v>
       </c>
       <c r="C3" s="14">
-        <f t="shared" ref="C3:C16" si="1">B3/A3</f>
+        <f t="shared" ref="C3:C17" si="1">B3/A3</f>
         <v>0.22500000000000001</v>
       </c>
       <c r="D3" s="3">
@@ -1679,18 +1679,20 @@
       <c r="I14" s="16">
         <v>0.91200000000000003</v>
       </c>
-      <c r="J14" s="16"/>
+      <c r="J14" s="16">
+        <v>0.98899999999999999</v>
+      </c>
       <c r="K14" s="12">
-        <f>0/60</f>
-        <v>0</v>
+        <f>734.58/60</f>
+        <v>12.243</v>
       </c>
       <c r="L14" s="12">
-        <f>0/60</f>
-        <v>0</v>
+        <f>15406.02/60</f>
+        <v>256.767</v>
       </c>
       <c r="M14" s="18">
-        <f>0/60</f>
-        <v>0</v>
+        <f>28.26/60</f>
+        <v>0.47100000000000003</v>
       </c>
       <c r="N14" s="2">
         <v>125</v>
@@ -1768,18 +1770,20 @@
       <c r="I15" s="16">
         <v>0.91</v>
       </c>
-      <c r="J15" s="16"/>
+      <c r="J15" s="16">
+        <v>0.879</v>
+      </c>
       <c r="K15" s="12">
-        <f>0/60</f>
-        <v>0</v>
+        <f>1017.62/60</f>
+        <v>16.960333333333335</v>
       </c>
       <c r="L15" s="12">
-        <f>0/60</f>
-        <v>0</v>
+        <f>21060.58/60</f>
+        <v>351.0096666666667</v>
       </c>
       <c r="M15" s="18">
-        <f>0/60</f>
-        <v>0</v>
+        <f>34.87/60</f>
+        <v>0.58116666666666661</v>
       </c>
       <c r="N15" s="2">
         <v>128</v>
@@ -1857,18 +1861,20 @@
       <c r="I16" s="16">
         <v>0.90900000000000003</v>
       </c>
-      <c r="J16" s="16"/>
+      <c r="J16" s="16">
+        <v>0.877</v>
+      </c>
       <c r="K16" s="12">
-        <f>0/60</f>
-        <v>0</v>
+        <f>1339.89/60</f>
+        <v>22.331500000000002</v>
       </c>
       <c r="L16" s="12">
-        <f>0/60</f>
-        <v>0</v>
+        <f>39843.97/60</f>
+        <v>664.06616666666673</v>
       </c>
       <c r="M16" s="18">
-        <f>0/60</f>
-        <v>0</v>
+        <f>47.47/60</f>
+        <v>0.79116666666666668</v>
       </c>
       <c r="N16" s="2">
         <v>129</v>
@@ -1920,28 +1926,50 @@
         <f t="shared" si="2"/>
         <v>520000</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+      <c r="B17" s="2">
+        <f>A17-D17</f>
+        <v>148330</v>
+      </c>
+      <c r="C17" s="17">
+        <f t="shared" si="1"/>
+        <v>0.28525</v>
+      </c>
+      <c r="D17" s="2">
+        <v>371670</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="G17" s="16">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="H17" s="16">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="I17" s="16">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="J17" s="16">
+        <v>0.874</v>
+      </c>
       <c r="K17" s="12">
-        <f>0/60</f>
-        <v>0</v>
+        <f>1672.72/60</f>
+        <v>27.878666666666668</v>
       </c>
       <c r="L17" s="12">
-        <f>0/60</f>
-        <v>0</v>
+        <f>33395.93/60</f>
+        <v>556.59883333333335</v>
       </c>
       <c r="M17" s="18">
-        <f>0/60</f>
-        <v>0</v>
-      </c>
-      <c r="N17" s="2"/>
+        <f>51.26/60</f>
+        <v>0.85433333333333328</v>
+      </c>
+      <c r="N17" s="2">
+        <v>130</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>

</xml_diff>

<commit_message>
[RCE] Update data for 585000 rows of data
</commit_message>
<xml_diff>
--- a/project/ExperimentRecord - Target Variable - Acceptable_Resolution_Status.xlsx
+++ b/project/ExperimentRecord - Target Variable - Acceptable_Resolution_Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\school\SPS\DATA622\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C4AD8B-F82A-4257-B7D8-A62ADE234CCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2C46C2-AF03-4953-AD49-0FD4488E9E91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="600" windowWidth="12300" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="945" windowWidth="12300" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -571,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC25"/>
+  <dimension ref="A1:BC26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="12" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f t="shared" ref="A12:A17" si="2">A11+65000</f>
+        <f t="shared" ref="A12:A18" si="2">A11+65000</f>
         <v>195000</v>
       </c>
       <c r="B12" s="2">
@@ -1972,53 +1972,103 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="A18" s="2">
+        <f t="shared" si="2"/>
+        <v>585000</v>
+      </c>
+      <c r="B18" s="2">
+        <f>A18-D18</f>
+        <v>168151</v>
+      </c>
+      <c r="C18" s="17">
+        <f t="shared" ref="C18" si="3">B18/A18</f>
+        <v>0.28743760683760683</v>
+      </c>
+      <c r="D18" s="2">
+        <v>416849</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="H18" s="16">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I18" s="16">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="J18" s="16">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="K18" s="12">
+        <f>2024.97/60</f>
+        <v>33.749499999999998</v>
+      </c>
+      <c r="L18" s="12">
+        <f>61748.06/60</f>
+        <v>1029.1343333333332</v>
+      </c>
+      <c r="M18" s="18">
+        <f>60.24/60</f>
+        <v>1.004</v>
+      </c>
+      <c r="N18" s="2">
+        <v>131</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>